<commit_message>
Creation of text files for each request
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="7">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -362,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,10 +410,871 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>22</v>
-      </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>22</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>22</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>22</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>22</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>22</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>22</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62">
+        <v>22</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65">
+        <v>22</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>22</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>22</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>22</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <v>22</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>22</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>22</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>22</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89">
+        <v>22</v>
+      </c>
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>6</v>
+      </c>
+      <c r="C91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>3</v>
+      </c>
+      <c r="B92">
+        <v>22</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95">
+        <v>22</v>
+      </c>
+      <c r="C95" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98">
+        <v>22</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>